<commit_message>
i am off to sleep for a bit
</commit_message>
<xml_diff>
--- a/disgenet/disgenet_data.xlsx
+++ b/disgenet/disgenet_data.xlsx
@@ -5,17 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmarselis/src/db/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmarselis/src/db/disgenet/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="42240" windowHeight="19180" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="9000" yWindow="1440" windowWidth="42240" windowHeight="19180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="disgenet_data" sheetId="1" r:id="rId1"/>
     <sheet name="uniprotId" sheetId="2" r:id="rId2"/>
     <sheet name="list of proteins" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">disgenet_data!$A$1:$W$8</definedName>
+  </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="82">
   <si>
     <t>C0030567</t>
   </si>
@@ -79,9 +82,6 @@
     <t>P27338</t>
   </si>
   <si>
-    <t>monoamine oxidase B</t>
-  </si>
-  <si>
     <t>Metabolism</t>
   </si>
   <si>
@@ -254,13 +254,37 @@
   </si>
   <si>
     <t>sourceId</t>
+  </si>
+  <si>
+    <t>geneSymbol</t>
+  </si>
+  <si>
+    <t>SNCA</t>
+  </si>
+  <si>
+    <t>LRRK2</t>
+  </si>
+  <si>
+    <t>MAPT</t>
+  </si>
+  <si>
+    <t>PARK2</t>
+  </si>
+  <si>
+    <t>PINK1</t>
+  </si>
+  <si>
+    <t>MAOB</t>
+  </si>
+  <si>
+    <t>BST1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -272,6 +296,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -294,8 +334,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -306,7 +348,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -582,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,86 +646,90 @@
     <col min="10" max="10" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="28.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="24.6640625" style="1" customWidth="1"/>
-    <col min="16" max="18" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="28.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="24.6640625" style="1" customWidth="1"/>
+    <col min="17" max="19" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W1" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -713,43 +761,46 @@
         <v>7</v>
       </c>
       <c r="K2" s="1">
-        <v>683</v>
+        <v>6622</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S2" s="1">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="T2" s="1">
-        <v>6</v>
-      </c>
-      <c r="U2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="U2" s="1">
+        <v>4</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W2" s="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -781,43 +832,46 @@
         <v>7</v>
       </c>
       <c r="K3" s="1">
-        <v>4129</v>
+        <v>120892</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3" s="1">
-        <v>29</v>
+        <v>50</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="T3" s="1">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="U3" s="1">
+        <v>11</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W3" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -852,40 +906,43 @@
         <v>4137</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
         <v>58</v>
       </c>
-      <c r="T4" s="1">
+      <c r="U4" s="1">
         <v>6</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="1">
+      <c r="W4" s="1">
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -920,40 +977,43 @@
         <v>5071</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S5" s="1">
+      <c r="T5" s="1">
         <v>151</v>
       </c>
-      <c r="T5" s="1">
-        <v>0</v>
-      </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V5" s="1">
+      <c r="W5" s="1">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -985,43 +1045,46 @@
         <v>7</v>
       </c>
       <c r="K6" s="1">
-        <v>6622</v>
+        <v>65018</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S6" s="1">
-        <v>169</v>
+        <v>44</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="T6" s="1">
-        <v>4</v>
-      </c>
-      <c r="U6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="U6" s="1">
+        <v>3</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V6" s="1">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W6" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1053,43 +1116,43 @@
         <v>7</v>
       </c>
       <c r="K7" s="1">
-        <v>65018</v>
+        <v>4129</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S7" s="1">
-        <v>114</v>
+        <v>19</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="T7" s="1">
-        <v>3</v>
-      </c>
-      <c r="U7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0</v>
+      </c>
+      <c r="V7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V7" s="1">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W7" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1121,44 +1184,53 @@
         <v>7</v>
       </c>
       <c r="K8" s="1">
-        <v>120892</v>
+        <v>683</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="N8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="P8" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="S8" s="1">
-        <v>289</v>
+        <v>12</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="T8" s="1">
-        <v>11</v>
-      </c>
-      <c r="U8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U8" s="1">
+        <v>6</v>
+      </c>
+      <c r="V8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V8" s="1">
-        <v>74</v>
+      <c r="W8" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:W8">
+    <sortState ref="A2:W8">
+      <sortCondition descending="1" ref="S1:S8"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1177,7 +1249,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -1192,27 +1264,27 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1224,7 +1296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView showRuler="0" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -1245,27 +1317,27 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>